<commit_message>
created Registration Builder class
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testdata.xlsx
+++ b/src/test/resources/testData/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="84" windowWidth="13332" windowHeight="5544"/>
+    <workbookView xWindow="480" yWindow="84" windowWidth="13332" windowHeight="5544" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="154">
   <si>
     <t>Password_Incorrect</t>
   </si>
@@ -912,7 +912,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="204">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1497,6 +1497,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1796,7 +1802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -1964,9 +1970,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M3" sqref="L3:M3"/>
+      <selection pane="bottomLeft" activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2002,7 +2008,7 @@
       <c r="D1" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="202" t="s">
         <v>63</v>
       </c>
       <c r="F1" s="22" t="s">
@@ -2047,8 +2053,8 @@
       <c r="D2" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="131">
-        <v>10101991</v>
+      <c r="E2" s="169" t="s">
+        <v>147</v>
       </c>
       <c r="F2" s="23" t="s">
         <v>75</v>
@@ -2092,7 +2098,7 @@
       <c r="D3" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="131">
+      <c r="E3" s="170">
         <v>10101991</v>
       </c>
       <c r="F3" s="23" t="s">
@@ -2137,8 +2143,8 @@
       <c r="D4" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="131">
-        <v>10101991</v>
+      <c r="E4" s="170" t="s">
+        <v>147</v>
       </c>
       <c r="F4" s="23" t="s">
         <v>75</v>
@@ -2180,8 +2186,8 @@
       <c r="D5" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="131">
-        <v>10101991</v>
+      <c r="E5" s="203" t="s">
+        <v>147</v>
       </c>
       <c r="F5" s="23" t="s">
         <v>75</v>
@@ -2223,8 +2229,8 @@
         <v>82</v>
       </c>
       <c r="D6" s="25"/>
-      <c r="E6" s="133">
-        <v>10101991</v>
+      <c r="E6" s="171" t="s">
+        <v>147</v>
       </c>
       <c r="F6" s="25" t="s">
         <v>75</v>
@@ -2268,8 +2274,8 @@
       <c r="D7" s="27">
         <v>456789456</v>
       </c>
-      <c r="E7" s="134">
-        <v>10101991</v>
+      <c r="E7" s="194" t="s">
+        <v>147</v>
       </c>
       <c r="F7" s="27" t="s">
         <v>75</v>
@@ -2311,8 +2317,8 @@
       <c r="D8" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="E8" s="134">
-        <v>10101991</v>
+      <c r="E8" s="194" t="s">
+        <v>147</v>
       </c>
       <c r="F8" s="27" t="s">
         <v>75</v>
@@ -2354,8 +2360,8 @@
       <c r="D9" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="135">
-        <v>10101991</v>
+      <c r="E9" s="195" t="s">
+        <v>147</v>
       </c>
       <c r="F9" s="30" t="s">
         <v>75</v>
@@ -2615,7 +2621,7 @@
       <c r="E15" s="179" t="s">
         <v>147</v>
       </c>
-      <c r="F15" s="33"/>
+      <c r="F15" s="136"/>
       <c r="G15" s="179" t="s">
         <v>143</v>
       </c>
@@ -2658,7 +2664,7 @@
       <c r="E16" s="180" t="s">
         <v>147</v>
       </c>
-      <c r="F16" s="33">
+      <c r="F16" s="137">
         <v>456789123</v>
       </c>
       <c r="G16" s="180" t="s">
@@ -2701,7 +2707,7 @@
       <c r="E17" s="181" t="s">
         <v>147</v>
       </c>
-      <c r="F17" s="36" t="s">
+      <c r="F17" s="138" t="s">
         <v>84</v>
       </c>
       <c r="G17" s="181" t="s">

</xml_diff>

<commit_message>
added productPage, cross browser testng and global context
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testdata.xlsx
+++ b/src/test/resources/testData/testdata.xlsx
@@ -912,7 +912,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="204">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -996,9 +996,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1303,9 +1300,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1841,7 +1835,7 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="200" t="s">
+      <c r="A3" s="198" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1855,7 +1849,7 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="200" t="s">
+      <c r="A4" s="198" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1869,7 +1863,7 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="200" t="s">
+      <c r="A5" s="198" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1883,7 +1877,7 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="200" t="s">
+      <c r="A6" s="198" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1897,7 +1891,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.6" thickBot="1">
-      <c r="A7" s="200" t="s">
+      <c r="A7" s="198" t="s">
         <v>153</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1911,45 +1905,45 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="162"/>
-      <c r="B8" s="163"/>
-      <c r="C8" s="164"/>
+      <c r="A8" s="160"/>
+      <c r="B8" s="161"/>
+      <c r="C8" s="162"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="165"/>
-      <c r="B9" s="166"/>
-      <c r="C9" s="167"/>
-      <c r="D9" s="168"/>
+      <c r="A9" s="163"/>
+      <c r="B9" s="164"/>
+      <c r="C9" s="165"/>
+      <c r="D9" s="166"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="165"/>
-      <c r="B10" s="166"/>
-      <c r="C10" s="167"/>
-      <c r="D10" s="168"/>
+      <c r="A10" s="163"/>
+      <c r="B10" s="164"/>
+      <c r="C10" s="165"/>
+      <c r="D10" s="166"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="165"/>
-      <c r="B11" s="166"/>
-      <c r="C11" s="167"/>
-      <c r="D11" s="168"/>
+      <c r="A11" s="163"/>
+      <c r="B11" s="164"/>
+      <c r="C11" s="165"/>
+      <c r="D11" s="166"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="165"/>
-      <c r="B12" s="198"/>
-      <c r="C12" s="199"/>
-      <c r="D12" s="201"/>
+      <c r="A12" s="163"/>
+      <c r="B12" s="196"/>
+      <c r="C12" s="197"/>
+      <c r="D12" s="199"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="165"/>
-      <c r="B13" s="166"/>
-      <c r="C13" s="167"/>
-      <c r="D13" s="168"/>
+      <c r="A13" s="163"/>
+      <c r="B13" s="164"/>
+      <c r="C13" s="165"/>
+      <c r="D13" s="166"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="165"/>
-      <c r="B14" s="165"/>
-      <c r="C14" s="167"/>
-      <c r="D14" s="168"/>
+      <c r="A14" s="163"/>
+      <c r="B14" s="163"/>
+      <c r="C14" s="165"/>
+      <c r="D14" s="166"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1971,8 +1965,8 @@
   <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2008,7 +2002,7 @@
       <c r="D1" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="202" t="s">
+      <c r="E1" s="200" t="s">
         <v>63</v>
       </c>
       <c r="F1" s="22" t="s">
@@ -2046,175 +2040,175 @@
       <c r="A2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="103" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="131"/>
+      <c r="B2" s="102" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="130"/>
       <c r="D2" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="169" t="s">
+      <c r="E2" s="167" t="s">
         <v>147</v>
       </c>
       <c r="F2" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="169" t="s">
+      <c r="G2" s="167" t="s">
         <v>143</v>
       </c>
       <c r="H2" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="I2" s="160" t="s">
+      <c r="I2" s="158" t="s">
         <v>73</v>
       </c>
       <c r="J2" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="K2" s="169" t="s">
+      <c r="K2" s="167" t="s">
         <v>140</v>
       </c>
       <c r="L2" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="M2" s="160" t="s">
+      <c r="M2" s="158" t="s">
         <v>118</v>
       </c>
       <c r="N2" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="O2" s="196"/>
+      <c r="O2" s="194"/>
     </row>
     <row r="3" spans="1:15" ht="15">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="79" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="131">
+      <c r="C3" s="130">
         <v>456789456</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="170">
+      <c r="E3" s="168">
         <v>10101991</v>
       </c>
       <c r="F3" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="G3" s="170" t="s">
+      <c r="G3" s="168" t="s">
         <v>143</v>
       </c>
       <c r="H3" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="I3" s="131" t="s">
+      <c r="I3" s="130" t="s">
         <v>73</v>
       </c>
       <c r="J3" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="K3" s="170" t="s">
+      <c r="K3" s="168" t="s">
         <v>141</v>
       </c>
       <c r="L3" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="M3" s="131" t="s">
+      <c r="M3" s="130" t="s">
         <v>119</v>
       </c>
-      <c r="N3" s="196"/>
-      <c r="O3" s="196" t="s">
+      <c r="N3" s="194"/>
+      <c r="O3" s="194" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="79" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="132" t="s">
-        <v>80</v>
+      <c r="C4" s="148" t="s">
+        <v>96</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="170" t="s">
+      <c r="E4" s="168" t="s">
         <v>147</v>
       </c>
       <c r="F4" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="170" t="s">
+      <c r="G4" s="168" t="s">
         <v>143</v>
       </c>
       <c r="H4" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="I4" s="131" t="s">
+      <c r="I4" s="130" t="s">
         <v>73</v>
       </c>
       <c r="J4" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="K4" s="170" t="s">
+      <c r="K4" s="168" t="s">
         <v>141</v>
       </c>
       <c r="L4" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="M4" s="131" t="s">
+      <c r="M4" s="130" t="s">
         <v>120</v>
       </c>
-      <c r="N4" s="196"/>
-      <c r="O4" s="196"/>
+      <c r="N4" s="194"/>
+      <c r="O4" s="194"/>
     </row>
     <row r="5" spans="1:15" ht="15.6" thickBot="1">
-      <c r="A5" s="102" t="s">
+      <c r="A5" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="104" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="131" t="s">
+      <c r="B5" s="103" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="130" t="s">
         <v>81</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="203" t="s">
+      <c r="E5" s="201" t="s">
         <v>147</v>
       </c>
       <c r="F5" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="G5" s="170" t="s">
+      <c r="G5" s="168" t="s">
         <v>143</v>
       </c>
       <c r="H5" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="I5" s="131" t="s">
+      <c r="I5" s="130" t="s">
         <v>73</v>
       </c>
       <c r="J5" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="K5" s="170" t="s">
+      <c r="K5" s="168" t="s">
         <v>141</v>
       </c>
       <c r="L5" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="M5" s="131" t="s">
+      <c r="M5" s="130" t="s">
         <v>121</v>
       </c>
-      <c r="N5" s="196"/>
-      <c r="O5" s="196" t="s">
+      <c r="N5" s="194"/>
+      <c r="O5" s="194" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2222,2051 +2216,2051 @@
       <c r="A6" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="86" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="133" t="s">
+      <c r="B6" s="85" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="131" t="s">
         <v>82</v>
       </c>
       <c r="D6" s="25"/>
-      <c r="E6" s="171" t="s">
+      <c r="E6" s="169" t="s">
         <v>147</v>
       </c>
       <c r="F6" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="G6" s="171" t="s">
+      <c r="G6" s="169" t="s">
         <v>143</v>
       </c>
       <c r="H6" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="I6" s="133" t="s">
+      <c r="I6" s="131" t="s">
         <v>73</v>
       </c>
       <c r="J6" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="K6" s="133" t="s">
+      <c r="K6" s="131" t="s">
         <v>141</v>
       </c>
       <c r="L6" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="M6" s="133" t="s">
+      <c r="M6" s="131" t="s">
         <v>118</v>
       </c>
       <c r="N6" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="O6" s="196"/>
+      <c r="O6" s="194"/>
     </row>
     <row r="7" spans="1:15" ht="15">
-      <c r="A7" s="81" t="s">
+      <c r="A7" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="105" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="134" t="s">
+      <c r="B7" s="104" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="132" t="s">
         <v>82</v>
       </c>
       <c r="D7" s="27">
         <v>456789456</v>
       </c>
-      <c r="E7" s="194" t="s">
+      <c r="E7" s="192" t="s">
         <v>147</v>
       </c>
       <c r="F7" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="G7" s="194" t="s">
+      <c r="G7" s="192" t="s">
         <v>143</v>
       </c>
       <c r="H7" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="I7" s="134" t="s">
+      <c r="I7" s="132" t="s">
         <v>73</v>
       </c>
       <c r="J7" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="K7" s="134" t="s">
+      <c r="K7" s="132" t="s">
         <v>141</v>
       </c>
       <c r="L7" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="M7" s="134" t="s">
+      <c r="M7" s="132" t="s">
         <v>119</v>
       </c>
-      <c r="N7" s="196"/>
-      <c r="O7" s="196"/>
+      <c r="N7" s="194"/>
+      <c r="O7" s="194"/>
     </row>
     <row r="8" spans="1:15" ht="15">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="105" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="134" t="s">
-        <v>82</v>
-      </c>
-      <c r="D8" s="29" t="s">
+      <c r="B8" s="104" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="132" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="148" t="s">
         <v>80</v>
       </c>
-      <c r="E8" s="194" t="s">
+      <c r="E8" s="192" t="s">
         <v>147</v>
       </c>
       <c r="F8" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="G8" s="194" t="s">
+      <c r="G8" s="192" t="s">
         <v>143</v>
       </c>
       <c r="H8" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="I8" s="134" t="s">
+      <c r="I8" s="132" t="s">
         <v>73</v>
       </c>
       <c r="J8" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="K8" s="134" t="s">
+      <c r="K8" s="132" t="s">
         <v>141</v>
       </c>
       <c r="L8" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="M8" s="134" t="s">
+      <c r="M8" s="132" t="s">
         <v>120</v>
       </c>
-      <c r="N8" s="196"/>
-      <c r="O8" s="196"/>
+      <c r="N8" s="194"/>
+      <c r="O8" s="194"/>
     </row>
     <row r="9" spans="1:15" ht="15.6" thickBot="1">
-      <c r="A9" s="101" t="s">
+      <c r="A9" s="100" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="135" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" s="30" t="s">
+      <c r="C9" s="133" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="195" t="s">
+      <c r="E9" s="193" t="s">
         <v>147</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="G9" s="195" t="s">
+      <c r="G9" s="193" t="s">
         <v>143</v>
       </c>
-      <c r="H9" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="I9" s="135" t="s">
-        <v>73</v>
-      </c>
-      <c r="J9" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="K9" s="135" t="s">
+      <c r="H9" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="I9" s="133" t="s">
+        <v>73</v>
+      </c>
+      <c r="J9" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="K9" s="133" t="s">
         <v>141</v>
       </c>
-      <c r="L9" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="M9" s="135" t="s">
+      <c r="L9" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="M9" s="133" t="s">
         <v>121</v>
       </c>
-      <c r="N9" s="196"/>
-      <c r="O9" s="196"/>
+      <c r="N9" s="194"/>
+      <c r="O9" s="194"/>
     </row>
     <row r="10" spans="1:15" ht="15">
       <c r="A10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="103" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="131" t="s">
+      <c r="B10" s="102" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="130" t="s">
         <v>82</v>
       </c>
       <c r="D10" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="131"/>
+      <c r="E10" s="130"/>
       <c r="F10" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="G10" s="170" t="s">
+      <c r="G10" s="168" t="s">
         <v>143</v>
       </c>
       <c r="H10" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="I10" s="131" t="s">
+      <c r="I10" s="130" t="s">
         <v>73</v>
       </c>
       <c r="J10" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="K10" s="160" t="s">
+      <c r="K10" s="158" t="s">
         <v>141</v>
       </c>
       <c r="L10" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="M10" s="131" t="s">
+      <c r="M10" s="130" t="s">
         <v>118</v>
       </c>
       <c r="N10" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="O10" s="196"/>
+      <c r="O10" s="194"/>
     </row>
     <row r="11" spans="1:15" ht="15">
-      <c r="A11" s="80" t="s">
+      <c r="A11" s="79" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="131" t="s">
+      <c r="C11" s="130" t="s">
         <v>82</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="131" t="s">
+      <c r="E11" s="130" t="s">
         <v>83</v>
       </c>
       <c r="F11" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="G11" s="170" t="s">
+      <c r="G11" s="168" t="s">
         <v>143</v>
       </c>
       <c r="H11" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="I11" s="131" t="s">
+      <c r="I11" s="130" t="s">
         <v>73</v>
       </c>
       <c r="J11" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="K11" s="131" t="s">
+      <c r="K11" s="130" t="s">
         <v>141</v>
       </c>
       <c r="L11" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="M11" s="131" t="s">
+      <c r="M11" s="130" t="s">
         <v>119</v>
       </c>
-      <c r="N11" s="196"/>
-      <c r="O11" s="196"/>
+      <c r="N11" s="194"/>
+      <c r="O11" s="194"/>
     </row>
     <row r="12" spans="1:15" ht="15">
-      <c r="A12" s="80" t="s">
+      <c r="A12" s="79" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="131" t="s">
+      <c r="C12" s="130" t="s">
         <v>82</v>
       </c>
       <c r="D12" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="131" t="s">
+      <c r="E12" s="130" t="s">
         <v>84</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="G12" s="170" t="s">
+      <c r="G12" s="168" t="s">
         <v>143</v>
       </c>
       <c r="H12" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="I12" s="131" t="s">
+      <c r="I12" s="130" t="s">
         <v>73</v>
       </c>
       <c r="J12" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="K12" s="131" t="s">
+      <c r="K12" s="130" t="s">
         <v>141</v>
       </c>
       <c r="L12" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="M12" s="131" t="s">
+      <c r="M12" s="130" t="s">
         <v>120</v>
       </c>
-      <c r="N12" s="196"/>
-      <c r="O12" s="196"/>
+      <c r="N12" s="194"/>
+      <c r="O12" s="194"/>
     </row>
     <row r="13" spans="1:15" ht="15">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="79" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="131" t="s">
+      <c r="C13" s="130" t="s">
         <v>82</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E13" s="131" t="s">
+      <c r="E13" s="130" t="s">
         <v>85</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="G13" s="170" t="s">
+      <c r="G13" s="168" t="s">
         <v>143</v>
       </c>
       <c r="H13" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="I13" s="131" t="s">
+      <c r="I13" s="130" t="s">
         <v>73</v>
       </c>
       <c r="J13" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="K13" s="131" t="s">
+      <c r="K13" s="130" t="s">
         <v>141</v>
       </c>
       <c r="L13" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="M13" s="131" t="s">
+      <c r="M13" s="130" t="s">
         <v>121</v>
       </c>
-      <c r="N13" s="196"/>
-      <c r="O13" s="196"/>
+      <c r="N13" s="194"/>
+      <c r="O13" s="194"/>
     </row>
     <row r="14" spans="1:15" ht="15.6" thickBot="1">
       <c r="A14" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="104" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="131" t="s">
+      <c r="B14" s="103" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="130" t="s">
         <v>82</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="170" t="s">
+      <c r="E14" s="168" t="s">
         <v>146</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="G14" s="170" t="s">
+      <c r="G14" s="168" t="s">
         <v>143</v>
       </c>
       <c r="H14" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="I14" s="131" t="s">
+      <c r="I14" s="130" t="s">
         <v>73</v>
       </c>
       <c r="J14" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="K14" s="178" t="s">
+      <c r="K14" s="176" t="s">
         <v>141</v>
       </c>
       <c r="L14" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="M14" s="131" t="s">
+      <c r="M14" s="130" t="s">
         <v>122</v>
       </c>
-      <c r="N14" s="196"/>
-      <c r="O14" s="196"/>
+      <c r="N14" s="194"/>
+      <c r="O14" s="194"/>
     </row>
     <row r="15" spans="1:15" ht="15">
-      <c r="A15" s="99" t="s">
+      <c r="A15" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="106" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="136" t="s">
-        <v>82</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="179" t="s">
+      <c r="B15" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="134" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="177" t="s">
         <v>147</v>
       </c>
-      <c r="F15" s="136"/>
-      <c r="G15" s="179" t="s">
+      <c r="F15" s="134"/>
+      <c r="G15" s="177" t="s">
         <v>143</v>
       </c>
-      <c r="H15" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="I15" s="136" t="s">
-        <v>73</v>
-      </c>
-      <c r="J15" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="K15" s="136" t="s">
+      <c r="H15" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="I15" s="134" t="s">
+        <v>73</v>
+      </c>
+      <c r="J15" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="K15" s="134" t="s">
         <v>141</v>
       </c>
-      <c r="L15" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="M15" s="136" t="s">
+      <c r="L15" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="M15" s="134" t="s">
         <v>118</v>
       </c>
       <c r="N15" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="O15" s="196"/>
+      <c r="O15" s="194"/>
     </row>
     <row r="16" spans="1:15" ht="15">
-      <c r="A16" s="82" t="s">
+      <c r="A16" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="107" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="D16" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="E16" s="180" t="s">
+      <c r="B16" s="106" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="135" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="178" t="s">
         <v>147</v>
       </c>
-      <c r="F16" s="137">
+      <c r="F16" s="135">
         <v>456789123</v>
       </c>
-      <c r="G16" s="180" t="s">
+      <c r="G16" s="178" t="s">
         <v>143</v>
       </c>
-      <c r="H16" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="I16" s="137" t="s">
-        <v>73</v>
-      </c>
-      <c r="J16" s="33" t="s">
-        <v>116</v>
-      </c>
-      <c r="K16" s="137" t="s">
+      <c r="H16" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="I16" s="135" t="s">
+        <v>73</v>
+      </c>
+      <c r="J16" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="K16" s="135" t="s">
         <v>141</v>
       </c>
-      <c r="L16" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="M16" s="137" t="s">
+      <c r="L16" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="M16" s="135" t="s">
         <v>119</v>
       </c>
-      <c r="N16" s="196"/>
-      <c r="O16" s="196"/>
+      <c r="N16" s="194"/>
+      <c r="O16" s="194"/>
     </row>
     <row r="17" spans="1:15" ht="15.6" thickBot="1">
-      <c r="A17" s="100" t="s">
+      <c r="A17" s="99" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="108" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="138" t="s">
-        <v>82</v>
-      </c>
-      <c r="D17" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" s="181" t="s">
+      <c r="B17" s="107" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="136" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="179" t="s">
         <v>147</v>
       </c>
-      <c r="F17" s="138" t="s">
+      <c r="F17" s="136" t="s">
         <v>84</v>
       </c>
-      <c r="G17" s="181" t="s">
+      <c r="G17" s="179" t="s">
         <v>143</v>
       </c>
-      <c r="H17" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="I17" s="138" t="s">
-        <v>73</v>
-      </c>
-      <c r="J17" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="K17" s="138" t="s">
+      <c r="H17" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="I17" s="136" t="s">
+        <v>73</v>
+      </c>
+      <c r="J17" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="K17" s="136" t="s">
         <v>141</v>
       </c>
-      <c r="L17" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="M17" s="138" t="s">
+      <c r="L17" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="M17" s="136" t="s">
         <v>120</v>
       </c>
-      <c r="N17" s="196"/>
-      <c r="O17" s="196"/>
+      <c r="N17" s="194"/>
+      <c r="O17" s="194"/>
     </row>
     <row r="18" spans="1:15" ht="15.6" thickBot="1">
       <c r="A18" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="109" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="D18" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="E18" s="193" t="s">
+      <c r="B18" s="108" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="137" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="191" t="s">
         <v>147</v>
       </c>
-      <c r="F18" s="38" t="s">
+      <c r="F18" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="G18" s="139"/>
-      <c r="H18" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="I18" s="139" t="s">
-        <v>73</v>
-      </c>
-      <c r="J18" s="38" t="s">
-        <v>116</v>
-      </c>
-      <c r="K18" s="139" t="s">
+      <c r="G18" s="137"/>
+      <c r="H18" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="I18" s="137" t="s">
+        <v>73</v>
+      </c>
+      <c r="J18" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="K18" s="137" t="s">
         <v>141</v>
       </c>
-      <c r="L18" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="M18" s="139" t="s">
+      <c r="L18" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="M18" s="137" t="s">
         <v>122</v>
       </c>
       <c r="N18" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="O18" s="196"/>
+      <c r="O18" s="194"/>
     </row>
     <row r="19" spans="1:15" ht="15">
-      <c r="A19" s="83" t="s">
+      <c r="A19" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="110" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="140" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="E19" s="182" t="s">
+      <c r="B19" s="109" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="138" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="180" t="s">
         <v>147</v>
       </c>
-      <c r="F19" s="40" t="s">
+      <c r="F19" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="G19" s="140" t="s">
+      <c r="G19" s="138" t="s">
         <v>86</v>
       </c>
-      <c r="H19" s="40" t="s">
-        <v>72</v>
-      </c>
-      <c r="I19" s="140" t="s">
-        <v>73</v>
-      </c>
-      <c r="J19" s="40" t="s">
-        <v>116</v>
-      </c>
-      <c r="K19" s="140" t="s">
+      <c r="H19" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" s="138" t="s">
+        <v>73</v>
+      </c>
+      <c r="J19" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="K19" s="138" t="s">
         <v>141</v>
       </c>
-      <c r="L19" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="M19" s="140" t="s">
+      <c r="L19" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="M19" s="138" t="s">
         <v>123</v>
       </c>
-      <c r="N19" s="196"/>
-      <c r="O19" s="196"/>
+      <c r="N19" s="194"/>
+      <c r="O19" s="194"/>
     </row>
     <row r="20" spans="1:15" ht="15">
-      <c r="A20" s="83" t="s">
+      <c r="A20" s="82" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="111" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="140" t="s">
-        <v>82</v>
-      </c>
-      <c r="D20" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" s="182" t="s">
+      <c r="B20" s="110" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="138" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="180" t="s">
         <v>147</v>
       </c>
-      <c r="F20" s="40" t="s">
+      <c r="F20" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="G20" s="140" t="s">
+      <c r="G20" s="138" t="s">
         <v>87</v>
       </c>
-      <c r="H20" s="40" t="s">
-        <v>72</v>
-      </c>
-      <c r="I20" s="140" t="s">
-        <v>73</v>
-      </c>
-      <c r="J20" s="40" t="s">
-        <v>116</v>
-      </c>
-      <c r="K20" s="140" t="s">
+      <c r="H20" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="I20" s="138" t="s">
+        <v>73</v>
+      </c>
+      <c r="J20" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="K20" s="138" t="s">
         <v>141</v>
       </c>
-      <c r="L20" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="M20" s="140" t="s">
+      <c r="L20" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="M20" s="138" t="s">
         <v>124</v>
       </c>
-      <c r="N20" s="196"/>
-      <c r="O20" s="196"/>
+      <c r="N20" s="194"/>
+      <c r="O20" s="194"/>
     </row>
     <row r="21" spans="1:15" ht="15">
-      <c r="A21" s="83" t="s">
+      <c r="A21" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="111" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="140" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" s="182" t="s">
+      <c r="B21" s="110" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="138" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="180" t="s">
         <v>147</v>
       </c>
-      <c r="F21" s="40" t="s">
+      <c r="F21" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="G21" s="140" t="s">
+      <c r="G21" s="138" t="s">
         <v>88</v>
       </c>
-      <c r="H21" s="40" t="s">
-        <v>72</v>
-      </c>
-      <c r="I21" s="140" t="s">
-        <v>73</v>
-      </c>
-      <c r="J21" s="40" t="s">
-        <v>116</v>
-      </c>
-      <c r="K21" s="140" t="s">
+      <c r="H21" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="I21" s="138" t="s">
+        <v>73</v>
+      </c>
+      <c r="J21" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="K21" s="138" t="s">
         <v>141</v>
       </c>
-      <c r="L21" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="M21" s="140" t="s">
+      <c r="L21" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="M21" s="138" t="s">
         <v>125</v>
       </c>
-      <c r="N21" s="196"/>
-      <c r="O21" s="196"/>
+      <c r="N21" s="194"/>
+      <c r="O21" s="194"/>
     </row>
     <row r="22" spans="1:15" ht="15">
-      <c r="A22" s="83" t="s">
+      <c r="A22" s="82" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="111" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="140" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="E22" s="182" t="s">
+      <c r="B22" s="110" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="138" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="180" t="s">
         <v>147</v>
       </c>
-      <c r="F22" s="40" t="s">
+      <c r="F22" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="G22" s="182" t="s">
+      <c r="G22" s="180" t="s">
         <v>144</v>
       </c>
-      <c r="H22" s="40" t="s">
-        <v>72</v>
-      </c>
-      <c r="I22" s="140" t="s">
-        <v>73</v>
-      </c>
-      <c r="J22" s="40" t="s">
-        <v>116</v>
-      </c>
-      <c r="K22" s="140" t="s">
+      <c r="H22" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="I22" s="138" t="s">
+        <v>73</v>
+      </c>
+      <c r="J22" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="K22" s="138" t="s">
         <v>141</v>
       </c>
-      <c r="L22" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="M22" s="140" t="s">
+      <c r="L22" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="M22" s="138" t="s">
         <v>126</v>
       </c>
-      <c r="N22" s="196"/>
-      <c r="O22" s="196"/>
+      <c r="N22" s="194"/>
+      <c r="O22" s="194"/>
     </row>
     <row r="23" spans="1:15" ht="15.6" thickBot="1">
       <c r="A23" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="112" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="141" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" s="183" t="s">
+      <c r="B23" s="111" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="139" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="181" t="s">
         <v>147</v>
       </c>
-      <c r="F23" s="42" t="s">
+      <c r="F23" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="G23" s="183" t="s">
+      <c r="G23" s="181" t="s">
         <v>145</v>
       </c>
-      <c r="H23" s="42" t="s">
-        <v>72</v>
-      </c>
-      <c r="I23" s="141" t="s">
-        <v>73</v>
-      </c>
-      <c r="J23" s="42" t="s">
-        <v>116</v>
-      </c>
-      <c r="K23" s="141" t="s">
+      <c r="H23" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="I23" s="139" t="s">
+        <v>73</v>
+      </c>
+      <c r="J23" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="K23" s="139" t="s">
         <v>141</v>
       </c>
-      <c r="L23" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="M23" s="141" t="s">
+      <c r="L23" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="M23" s="139" t="s">
         <v>127</v>
       </c>
-      <c r="N23" s="196"/>
-      <c r="O23" s="196"/>
+      <c r="N23" s="194"/>
+      <c r="O23" s="194"/>
     </row>
     <row r="24" spans="1:15" ht="15">
       <c r="A24" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="113" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="142" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" s="44" t="s">
-        <v>71</v>
-      </c>
-      <c r="E24" s="184" t="s">
+      <c r="B24" s="112" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="140" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="182" t="s">
         <v>147</v>
       </c>
-      <c r="F24" s="44" t="s">
+      <c r="F24" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="G24" s="184" t="s">
+      <c r="G24" s="182" t="s">
         <v>143</v>
       </c>
-      <c r="H24" s="44"/>
-      <c r="I24" s="142" t="s">
-        <v>73</v>
-      </c>
-      <c r="J24" s="44" t="s">
-        <v>116</v>
-      </c>
-      <c r="K24" s="142" t="s">
+      <c r="H24" s="43"/>
+      <c r="I24" s="140" t="s">
+        <v>73</v>
+      </c>
+      <c r="J24" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="K24" s="140" t="s">
         <v>141</v>
       </c>
-      <c r="L24" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="M24" s="142" t="s">
+      <c r="L24" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="M24" s="140" t="s">
         <v>122</v>
       </c>
       <c r="N24" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="O24" s="196"/>
+      <c r="O24" s="194"/>
     </row>
     <row r="25" spans="1:15" ht="15">
-      <c r="A25" s="84" t="s">
+      <c r="A25" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="114" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="143" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" s="46" t="s">
-        <v>71</v>
-      </c>
-      <c r="E25" s="185" t="s">
+      <c r="B25" s="113" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="141" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="183" t="s">
         <v>147</v>
       </c>
-      <c r="F25" s="46" t="s">
+      <c r="F25" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="G25" s="185" t="s">
+      <c r="G25" s="183" t="s">
         <v>143</v>
       </c>
-      <c r="H25" s="46">
+      <c r="H25" s="45">
         <v>456789</v>
       </c>
-      <c r="I25" s="143" t="s">
-        <v>73</v>
-      </c>
-      <c r="J25" s="46" t="s">
-        <v>116</v>
-      </c>
-      <c r="K25" s="143" t="s">
+      <c r="I25" s="141" t="s">
+        <v>73</v>
+      </c>
+      <c r="J25" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="K25" s="141" t="s">
         <v>141</v>
       </c>
-      <c r="L25" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="M25" s="143" t="s">
+      <c r="L25" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="M25" s="141" t="s">
         <v>123</v>
       </c>
-      <c r="N25" s="196"/>
-      <c r="O25" s="196"/>
+      <c r="N25" s="194"/>
+      <c r="O25" s="194"/>
     </row>
     <row r="26" spans="1:15" ht="15">
-      <c r="A26" s="84" t="s">
+      <c r="A26" s="83" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="114" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="143" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26" s="46" t="s">
-        <v>71</v>
-      </c>
-      <c r="E26" s="185" t="s">
+      <c r="B26" s="113" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="141" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="183" t="s">
         <v>147</v>
       </c>
-      <c r="F26" s="46" t="s">
+      <c r="F26" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="G26" s="185" t="s">
+      <c r="G26" s="183" t="s">
         <v>143</v>
       </c>
-      <c r="H26" s="47" t="s">
+      <c r="H26" s="148" t="s">
         <v>89</v>
       </c>
-      <c r="I26" s="143" t="s">
-        <v>73</v>
-      </c>
-      <c r="J26" s="46" t="s">
-        <v>116</v>
-      </c>
-      <c r="K26" s="143" t="s">
+      <c r="I26" s="141" t="s">
+        <v>73</v>
+      </c>
+      <c r="J26" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="K26" s="141" t="s">
         <v>141</v>
       </c>
-      <c r="L26" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="M26" s="143" t="s">
+      <c r="L26" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="M26" s="141" t="s">
         <v>124</v>
       </c>
-      <c r="N26" s="196"/>
-      <c r="O26" s="196"/>
+      <c r="N26" s="194"/>
+      <c r="O26" s="194"/>
     </row>
     <row r="27" spans="1:15" ht="15.6" thickBot="1">
       <c r="A27" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="115" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="144" t="s">
-        <v>82</v>
-      </c>
-      <c r="D27" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27" s="186" t="s">
+      <c r="B27" s="114" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="142" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" s="184" t="s">
         <v>147</v>
       </c>
-      <c r="F27" s="48" t="s">
+      <c r="F27" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="G27" s="186" t="s">
+      <c r="G27" s="184" t="s">
         <v>143</v>
       </c>
-      <c r="H27" s="48" t="s">
+      <c r="H27" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="I27" s="144" t="s">
-        <v>73</v>
-      </c>
-      <c r="J27" s="48" t="s">
-        <v>116</v>
-      </c>
-      <c r="K27" s="144" t="s">
+      <c r="I27" s="142" t="s">
+        <v>73</v>
+      </c>
+      <c r="J27" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="K27" s="142" t="s">
         <v>141</v>
       </c>
-      <c r="L27" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="M27" s="144" t="s">
+      <c r="L27" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="M27" s="142" t="s">
         <v>125</v>
       </c>
-      <c r="N27" s="196"/>
-      <c r="O27" s="196"/>
+      <c r="N27" s="194"/>
+      <c r="O27" s="194"/>
     </row>
     <row r="28" spans="1:15" ht="15">
-      <c r="A28" s="97" t="s">
+      <c r="A28" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="116" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="145" t="s">
-        <v>82</v>
-      </c>
-      <c r="D28" s="50" t="s">
-        <v>71</v>
-      </c>
-      <c r="E28" s="187" t="s">
+      <c r="B28" s="115" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="143" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" s="185" t="s">
         <v>147</v>
       </c>
-      <c r="F28" s="50" t="s">
+      <c r="F28" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="G28" s="187" t="s">
+      <c r="G28" s="185" t="s">
         <v>143</v>
       </c>
-      <c r="H28" s="50" t="s">
-        <v>72</v>
-      </c>
-      <c r="I28" s="145"/>
-      <c r="J28" s="50" t="s">
-        <v>116</v>
-      </c>
-      <c r="K28" s="145" t="s">
+      <c r="H28" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="I28" s="143"/>
+      <c r="J28" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="K28" s="143" t="s">
         <v>141</v>
       </c>
-      <c r="L28" s="51" t="s">
-        <v>74</v>
-      </c>
-      <c r="M28" s="145" t="s">
+      <c r="L28" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="M28" s="143" t="s">
         <v>122</v>
       </c>
       <c r="N28" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="O28" s="196"/>
+      <c r="O28" s="194"/>
     </row>
     <row r="29" spans="1:15" ht="15">
-      <c r="A29" s="85" t="s">
+      <c r="A29" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="117" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="146" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="E29" s="188" t="s">
+      <c r="B29" s="116" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="144" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29" s="186" t="s">
         <v>147</v>
       </c>
-      <c r="F29" s="52" t="s">
+      <c r="F29" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="G29" s="188" t="s">
+      <c r="G29" s="186" t="s">
         <v>143</v>
       </c>
-      <c r="H29" s="52" t="s">
-        <v>72</v>
-      </c>
-      <c r="I29" s="146">
+      <c r="H29" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="I29" s="144">
         <v>85</v>
       </c>
-      <c r="J29" s="52" t="s">
-        <v>116</v>
-      </c>
-      <c r="K29" s="146" t="s">
+      <c r="J29" s="51" t="s">
+        <v>116</v>
+      </c>
+      <c r="K29" s="144" t="s">
         <v>141</v>
       </c>
-      <c r="L29" s="53" t="s">
-        <v>74</v>
-      </c>
-      <c r="M29" s="146" t="s">
+      <c r="L29" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="M29" s="144" t="s">
         <v>123</v>
       </c>
-      <c r="N29" s="196"/>
-      <c r="O29" s="196"/>
+      <c r="N29" s="194"/>
+      <c r="O29" s="194"/>
     </row>
     <row r="30" spans="1:15" ht="15">
-      <c r="A30" s="85" t="s">
+      <c r="A30" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="117" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="146" t="s">
-        <v>82</v>
-      </c>
-      <c r="D30" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="E30" s="188" t="s">
+      <c r="B30" s="116" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="144" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" s="186" t="s">
         <v>147</v>
       </c>
-      <c r="F30" s="52" t="s">
+      <c r="F30" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="G30" s="188" t="s">
+      <c r="G30" s="186" t="s">
         <v>143</v>
       </c>
-      <c r="H30" s="52" t="s">
-        <v>72</v>
-      </c>
-      <c r="I30" s="146" t="s">
+      <c r="H30" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="I30" s="144" t="s">
         <v>91</v>
       </c>
-      <c r="J30" s="52" t="s">
-        <v>116</v>
-      </c>
-      <c r="K30" s="146" t="s">
+      <c r="J30" s="51" t="s">
+        <v>116</v>
+      </c>
+      <c r="K30" s="144" t="s">
         <v>141</v>
       </c>
-      <c r="L30" s="53" t="s">
-        <v>74</v>
-      </c>
-      <c r="M30" s="146" t="s">
+      <c r="L30" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="M30" s="144" t="s">
         <v>124</v>
       </c>
-      <c r="N30" s="196"/>
-      <c r="O30" s="196"/>
+      <c r="N30" s="194"/>
+      <c r="O30" s="194"/>
     </row>
     <row r="31" spans="1:15" ht="15.6" thickBot="1">
-      <c r="A31" s="98" t="s">
+      <c r="A31" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="118" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="147" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" s="54" t="s">
-        <v>71</v>
-      </c>
-      <c r="E31" s="189" t="s">
+      <c r="B31" s="117" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="145" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" s="187" t="s">
         <v>147</v>
       </c>
-      <c r="F31" s="54" t="s">
+      <c r="F31" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="G31" s="189" t="s">
+      <c r="G31" s="187" t="s">
         <v>143</v>
       </c>
-      <c r="H31" s="54" t="s">
-        <v>72</v>
-      </c>
-      <c r="I31" s="147" t="s">
+      <c r="H31" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="I31" s="145" t="s">
         <v>92</v>
       </c>
-      <c r="J31" s="54" t="s">
-        <v>116</v>
-      </c>
-      <c r="K31" s="147" t="s">
+      <c r="J31" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="K31" s="145" t="s">
         <v>141</v>
       </c>
-      <c r="L31" s="55" t="s">
-        <v>74</v>
-      </c>
-      <c r="M31" s="147" t="s">
+      <c r="L31" s="54" t="s">
+        <v>74</v>
+      </c>
+      <c r="M31" s="145" t="s">
         <v>125</v>
       </c>
-      <c r="N31" s="196"/>
-      <c r="O31" s="196"/>
+      <c r="N31" s="194"/>
+      <c r="O31" s="194"/>
     </row>
     <row r="32" spans="1:15" ht="15.6" thickBot="1">
       <c r="A32" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="119" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" s="148" t="s">
-        <v>82</v>
-      </c>
-      <c r="D32" s="56" t="s">
-        <v>71</v>
-      </c>
-      <c r="E32" s="190" t="s">
+      <c r="B32" s="118" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="146" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="E32" s="188" t="s">
         <v>147</v>
       </c>
-      <c r="F32" s="56" t="s">
+      <c r="F32" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="G32" s="190" t="s">
+      <c r="G32" s="188" t="s">
         <v>143</v>
       </c>
-      <c r="H32" s="56" t="s">
-        <v>72</v>
-      </c>
-      <c r="I32" s="148" t="s">
-        <v>73</v>
-      </c>
-      <c r="J32" s="56"/>
-      <c r="K32" s="148" t="s">
+      <c r="H32" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="I32" s="146" t="s">
+        <v>73</v>
+      </c>
+      <c r="J32" s="55"/>
+      <c r="K32" s="146" t="s">
         <v>141</v>
       </c>
-      <c r="L32" s="57" t="s">
-        <v>74</v>
-      </c>
-      <c r="M32" s="148" t="s">
+      <c r="L32" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="M32" s="146" t="s">
         <v>122</v>
       </c>
       <c r="N32" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="O32" s="196"/>
+      <c r="O32" s="194"/>
     </row>
     <row r="33" spans="1:15" ht="15">
-      <c r="A33" s="95" t="s">
+      <c r="A33" s="94" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="120" t="s">
-        <v>24</v>
-      </c>
-      <c r="C33" s="149" t="s">
-        <v>82</v>
-      </c>
-      <c r="D33" s="58" t="s">
-        <v>71</v>
-      </c>
-      <c r="E33" s="191" t="s">
+      <c r="B33" s="119" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="147" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="E33" s="189" t="s">
         <v>147</v>
       </c>
-      <c r="F33" s="58" t="s">
+      <c r="F33" s="57" t="s">
         <v>75</v>
       </c>
-      <c r="G33" s="191" t="s">
+      <c r="G33" s="189" t="s">
         <v>143</v>
       </c>
-      <c r="H33" s="58" t="s">
-        <v>72</v>
-      </c>
-      <c r="I33" s="149" t="s">
-        <v>73</v>
-      </c>
-      <c r="J33" s="58" t="s">
-        <v>116</v>
-      </c>
-      <c r="K33" s="149"/>
-      <c r="L33" s="59" t="s">
-        <v>74</v>
-      </c>
-      <c r="M33" s="149" t="s">
+      <c r="H33" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="I33" s="147" t="s">
+        <v>73</v>
+      </c>
+      <c r="J33" s="57" t="s">
+        <v>116</v>
+      </c>
+      <c r="K33" s="147"/>
+      <c r="L33" s="58" t="s">
+        <v>74</v>
+      </c>
+      <c r="M33" s="147" t="s">
         <v>122</v>
       </c>
       <c r="N33" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="O33" s="196"/>
+      <c r="O33" s="194"/>
     </row>
     <row r="34" spans="1:15" ht="15">
-      <c r="A34" s="87" t="s">
+      <c r="A34" s="86" t="s">
         <v>45</v>
       </c>
-      <c r="B34" s="121" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="150" t="s">
-        <v>82</v>
-      </c>
-      <c r="D34" s="60" t="s">
-        <v>71</v>
-      </c>
-      <c r="E34" s="192" t="s">
+      <c r="B34" s="120" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="148" t="s">
+        <v>82</v>
+      </c>
+      <c r="D34" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" s="190" t="s">
         <v>147</v>
       </c>
-      <c r="F34" s="60" t="s">
+      <c r="F34" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="G34" s="192" t="s">
+      <c r="G34" s="190" t="s">
         <v>143</v>
       </c>
-      <c r="H34" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="I34" s="150" t="s">
-        <v>73</v>
-      </c>
-      <c r="J34" s="60" t="s">
-        <v>116</v>
-      </c>
-      <c r="K34" s="150" t="s">
+      <c r="H34" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="I34" s="148" t="s">
+        <v>73</v>
+      </c>
+      <c r="J34" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="K34" s="148" t="s">
         <v>95</v>
       </c>
-      <c r="L34" s="61" t="s">
-        <v>74</v>
-      </c>
-      <c r="M34" s="150" t="s">
+      <c r="L34" s="60" t="s">
+        <v>74</v>
+      </c>
+      <c r="M34" s="148" t="s">
         <v>123</v>
       </c>
-      <c r="N34" s="196"/>
-      <c r="O34" s="196"/>
+      <c r="N34" s="194"/>
+      <c r="O34" s="194"/>
     </row>
     <row r="35" spans="1:15" ht="15">
-      <c r="A35" s="87" t="s">
+      <c r="A35" s="86" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="121" t="s">
-        <v>24</v>
-      </c>
-      <c r="C35" s="150" t="s">
-        <v>82</v>
-      </c>
-      <c r="D35" s="60" t="s">
-        <v>71</v>
-      </c>
-      <c r="E35" s="192" t="s">
+      <c r="B35" s="120" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="148" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="E35" s="190" t="s">
         <v>147</v>
       </c>
-      <c r="F35" s="60" t="s">
+      <c r="F35" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="G35" s="192" t="s">
+      <c r="G35" s="190" t="s">
         <v>143</v>
       </c>
-      <c r="H35" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="I35" s="150" t="s">
-        <v>73</v>
-      </c>
-      <c r="J35" s="60" t="s">
-        <v>116</v>
-      </c>
-      <c r="K35" s="150" t="s">
+      <c r="H35" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="I35" s="148" t="s">
+        <v>73</v>
+      </c>
+      <c r="J35" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="K35" s="148" t="s">
         <v>96</v>
       </c>
-      <c r="L35" s="61" t="s">
-        <v>74</v>
-      </c>
-      <c r="M35" s="150" t="s">
+      <c r="L35" s="60" t="s">
+        <v>74</v>
+      </c>
+      <c r="M35" s="148" t="s">
         <v>124</v>
       </c>
-      <c r="N35" s="196"/>
-      <c r="O35" s="196"/>
+      <c r="N35" s="194"/>
+      <c r="O35" s="194"/>
     </row>
     <row r="36" spans="1:15" ht="15">
-      <c r="A36" s="87" t="s">
+      <c r="A36" s="86" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="121" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36" s="150" t="s">
-        <v>82</v>
-      </c>
-      <c r="D36" s="60" t="s">
-        <v>71</v>
-      </c>
-      <c r="E36" s="192" t="s">
+      <c r="B36" s="120" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="148" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" s="190" t="s">
         <v>147</v>
       </c>
-      <c r="F36" s="60" t="s">
+      <c r="F36" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="G36" s="192" t="s">
+      <c r="G36" s="190" t="s">
         <v>143</v>
       </c>
-      <c r="H36" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="I36" s="150" t="s">
-        <v>73</v>
-      </c>
-      <c r="J36" s="60" t="s">
-        <v>116</v>
-      </c>
-      <c r="K36" s="150" t="s">
+      <c r="H36" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="I36" s="148" t="s">
+        <v>73</v>
+      </c>
+      <c r="J36" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="K36" s="148" t="s">
         <v>97</v>
       </c>
-      <c r="L36" s="61" t="s">
-        <v>74</v>
-      </c>
-      <c r="M36" s="150" t="s">
+      <c r="L36" s="60" t="s">
+        <v>74</v>
+      </c>
+      <c r="M36" s="148" t="s">
         <v>125</v>
       </c>
-      <c r="N36" s="196"/>
-      <c r="O36" s="196"/>
+      <c r="N36" s="194"/>
+      <c r="O36" s="194"/>
     </row>
     <row r="37" spans="1:15" ht="15">
-      <c r="A37" s="87" t="s">
+      <c r="A37" s="86" t="s">
         <v>48</v>
       </c>
-      <c r="B37" s="121" t="s">
-        <v>24</v>
-      </c>
-      <c r="C37" s="150" t="s">
-        <v>82</v>
-      </c>
-      <c r="D37" s="60" t="s">
-        <v>71</v>
-      </c>
-      <c r="E37" s="192" t="s">
+      <c r="B37" s="120" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="148" t="s">
+        <v>82</v>
+      </c>
+      <c r="D37" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="E37" s="190" t="s">
         <v>147</v>
       </c>
-      <c r="F37" s="60" t="s">
+      <c r="F37" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="G37" s="192" t="s">
+      <c r="G37" s="190" t="s">
         <v>143</v>
       </c>
-      <c r="H37" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="I37" s="150" t="s">
-        <v>73</v>
-      </c>
-      <c r="J37" s="60" t="s">
-        <v>116</v>
-      </c>
-      <c r="K37" s="150">
+      <c r="H37" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="I37" s="148" t="s">
+        <v>73</v>
+      </c>
+      <c r="J37" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="K37" s="148">
         <v>972865779</v>
       </c>
-      <c r="L37" s="61" t="s">
-        <v>74</v>
-      </c>
-      <c r="M37" s="150" t="s">
+      <c r="L37" s="60" t="s">
+        <v>74</v>
+      </c>
+      <c r="M37" s="148" t="s">
         <v>126</v>
       </c>
-      <c r="N37" s="196"/>
-      <c r="O37" s="196"/>
+      <c r="N37" s="194"/>
+      <c r="O37" s="194"/>
     </row>
     <row r="38" spans="1:15" ht="15">
-      <c r="A38" s="87" t="s">
+      <c r="A38" s="86" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="121" t="s">
-        <v>24</v>
-      </c>
-      <c r="C38" s="150" t="s">
-        <v>82</v>
-      </c>
-      <c r="D38" s="60" t="s">
-        <v>71</v>
-      </c>
-      <c r="E38" s="192" t="s">
+      <c r="B38" s="120" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="148" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="E38" s="190" t="s">
         <v>147</v>
       </c>
-      <c r="F38" s="60" t="s">
+      <c r="F38" s="59" t="s">
         <v>93</v>
       </c>
-      <c r="G38" s="192" t="s">
+      <c r="G38" s="190" t="s">
         <v>143</v>
       </c>
-      <c r="H38" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="I38" s="150" t="s">
-        <v>73</v>
-      </c>
-      <c r="J38" s="60" t="s">
-        <v>116</v>
-      </c>
-      <c r="K38" s="161" t="s">
+      <c r="H38" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="I38" s="148" t="s">
+        <v>73</v>
+      </c>
+      <c r="J38" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="K38" s="159" t="s">
         <v>98</v>
       </c>
-      <c r="L38" s="61" t="s">
-        <v>74</v>
-      </c>
-      <c r="M38" s="150" t="s">
+      <c r="L38" s="60" t="s">
+        <v>74</v>
+      </c>
+      <c r="M38" s="148" t="s">
         <v>127</v>
       </c>
-      <c r="N38" s="196"/>
-      <c r="O38" s="196"/>
+      <c r="N38" s="194"/>
+      <c r="O38" s="194"/>
     </row>
     <row r="39" spans="1:15" ht="15.6" thickBot="1">
-      <c r="A39" s="96" t="s">
+      <c r="A39" s="95" t="s">
         <v>50</v>
       </c>
-      <c r="B39" s="122" t="s">
-        <v>24</v>
-      </c>
-      <c r="C39" s="150" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" s="60" t="s">
-        <v>71</v>
-      </c>
-      <c r="E39" s="192" t="s">
+      <c r="B39" s="121" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="148" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="E39" s="190" t="s">
         <v>147</v>
       </c>
-      <c r="F39" s="60" t="s">
+      <c r="F39" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="G39" s="192" t="s">
+      <c r="G39" s="190" t="s">
         <v>143</v>
       </c>
-      <c r="H39" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="I39" s="150" t="s">
-        <v>73</v>
-      </c>
-      <c r="J39" s="60" t="s">
-        <v>116</v>
-      </c>
-      <c r="K39" s="150">
+      <c r="H39" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="I39" s="148" t="s">
+        <v>73</v>
+      </c>
+      <c r="J39" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="K39" s="148">
         <v>9999999999</v>
       </c>
-      <c r="L39" s="61" t="s">
-        <v>74</v>
-      </c>
-      <c r="M39" s="150" t="s">
+      <c r="L39" s="60" t="s">
+        <v>74</v>
+      </c>
+      <c r="M39" s="148" t="s">
         <v>128</v>
       </c>
-      <c r="N39" s="196"/>
-      <c r="O39" s="196"/>
+      <c r="N39" s="194"/>
+      <c r="O39" s="194"/>
     </row>
     <row r="40" spans="1:15" ht="15.6" thickBot="1">
-      <c r="A40" s="93" t="s">
+      <c r="A40" s="92" t="s">
         <v>51</v>
       </c>
-      <c r="B40" s="123" t="s">
-        <v>24</v>
-      </c>
-      <c r="C40" s="151" t="s">
-        <v>82</v>
-      </c>
-      <c r="D40" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="E40" s="172" t="s">
+      <c r="B40" s="122" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" s="149" t="s">
+        <v>82</v>
+      </c>
+      <c r="D40" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="E40" s="170" t="s">
         <v>147</v>
       </c>
-      <c r="F40" s="62" t="s">
+      <c r="F40" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="G40" s="172" t="s">
+      <c r="G40" s="170" t="s">
         <v>143</v>
       </c>
-      <c r="H40" s="62" t="s">
-        <v>72</v>
-      </c>
-      <c r="I40" s="151" t="s">
-        <v>73</v>
-      </c>
-      <c r="J40" s="62" t="s">
-        <v>116</v>
-      </c>
-      <c r="K40" s="172" t="s">
+      <c r="H40" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="I40" s="149" t="s">
+        <v>73</v>
+      </c>
+      <c r="J40" s="61" t="s">
+        <v>116</v>
+      </c>
+      <c r="K40" s="170" t="s">
         <v>142</v>
       </c>
-      <c r="L40" s="63"/>
-      <c r="M40" s="151" t="s">
+      <c r="L40" s="62"/>
+      <c r="M40" s="149" t="s">
         <v>124</v>
       </c>
       <c r="N40" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="O40" s="196"/>
+      <c r="O40" s="194"/>
     </row>
     <row r="41" spans="1:15" ht="15">
-      <c r="A41" s="93" t="s">
+      <c r="A41" s="92" t="s">
         <v>52</v>
       </c>
-      <c r="B41" s="124" t="s">
-        <v>24</v>
-      </c>
-      <c r="C41" s="152" t="s">
-        <v>82</v>
-      </c>
-      <c r="D41" s="64" t="s">
-        <v>71</v>
-      </c>
-      <c r="E41" s="173" t="s">
+      <c r="B41" s="123" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" s="150" t="s">
+        <v>82</v>
+      </c>
+      <c r="D41" s="63" t="s">
+        <v>71</v>
+      </c>
+      <c r="E41" s="171" t="s">
         <v>147</v>
       </c>
-      <c r="F41" s="64" t="s">
+      <c r="F41" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="G41" s="173" t="s">
+      <c r="G41" s="171" t="s">
         <v>143</v>
       </c>
-      <c r="H41" s="64" t="s">
-        <v>72</v>
-      </c>
-      <c r="I41" s="152" t="s">
-        <v>73</v>
-      </c>
-      <c r="J41" s="64" t="s">
-        <v>116</v>
-      </c>
-      <c r="K41" s="173" t="s">
+      <c r="H41" s="63" t="s">
+        <v>72</v>
+      </c>
+      <c r="I41" s="150" t="s">
+        <v>73</v>
+      </c>
+      <c r="J41" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="K41" s="171" t="s">
         <v>142</v>
       </c>
-      <c r="L41" s="65" t="s">
+      <c r="L41" s="64" t="s">
         <v>99</v>
       </c>
-      <c r="M41" s="152" t="s">
+      <c r="M41" s="150" t="s">
         <v>124</v>
       </c>
-      <c r="N41" s="196"/>
-      <c r="O41" s="196"/>
+      <c r="N41" s="194"/>
+      <c r="O41" s="194"/>
     </row>
     <row r="42" spans="1:15" ht="15.6" thickBot="1">
-      <c r="A42" s="94" t="s">
+      <c r="A42" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="B42" s="125" t="s">
-        <v>24</v>
-      </c>
-      <c r="C42" s="153" t="s">
-        <v>82</v>
-      </c>
-      <c r="D42" s="66" t="s">
-        <v>71</v>
-      </c>
-      <c r="E42" s="174" t="s">
+      <c r="B42" s="124" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" s="151" t="s">
+        <v>82</v>
+      </c>
+      <c r="D42" s="65" t="s">
+        <v>71</v>
+      </c>
+      <c r="E42" s="172" t="s">
         <v>147</v>
       </c>
-      <c r="F42" s="66" t="s">
+      <c r="F42" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="G42" s="174" t="s">
+      <c r="G42" s="172" t="s">
         <v>143</v>
       </c>
-      <c r="H42" s="66" t="s">
-        <v>72</v>
-      </c>
-      <c r="I42" s="153" t="s">
-        <v>73</v>
-      </c>
-      <c r="J42" s="66" t="s">
-        <v>116</v>
-      </c>
-      <c r="K42" s="174" t="s">
+      <c r="H42" s="65" t="s">
+        <v>72</v>
+      </c>
+      <c r="I42" s="151" t="s">
+        <v>73</v>
+      </c>
+      <c r="J42" s="65" t="s">
+        <v>116</v>
+      </c>
+      <c r="K42" s="172" t="s">
         <v>142</v>
       </c>
-      <c r="L42" s="67" t="s">
+      <c r="L42" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="M42" s="153" t="s">
+      <c r="M42" s="151" t="s">
         <v>127</v>
       </c>
-      <c r="N42" s="196"/>
-      <c r="O42" s="196"/>
+      <c r="N42" s="194"/>
+      <c r="O42" s="194"/>
     </row>
     <row r="43" spans="1:15" ht="15.6" thickBot="1">
-      <c r="A43" s="88" t="s">
+      <c r="A43" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="B43" s="126" t="s">
-        <v>24</v>
-      </c>
-      <c r="C43" s="154" t="s">
-        <v>82</v>
-      </c>
-      <c r="D43" s="68" t="s">
-        <v>71</v>
-      </c>
-      <c r="E43" s="175" t="s">
+      <c r="B43" s="125" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" s="152" t="s">
+        <v>82</v>
+      </c>
+      <c r="D43" s="67" t="s">
+        <v>71</v>
+      </c>
+      <c r="E43" s="173" t="s">
         <v>147</v>
       </c>
-      <c r="F43" s="68" t="s">
+      <c r="F43" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="G43" s="175" t="s">
+      <c r="G43" s="173" t="s">
         <v>143</v>
       </c>
-      <c r="H43" s="68" t="s">
-        <v>72</v>
-      </c>
-      <c r="I43" s="154" t="s">
-        <v>73</v>
-      </c>
-      <c r="J43" s="68" t="s">
-        <v>116</v>
-      </c>
-      <c r="K43" s="175" t="s">
+      <c r="H43" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="I43" s="152" t="s">
+        <v>73</v>
+      </c>
+      <c r="J43" s="67" t="s">
+        <v>116</v>
+      </c>
+      <c r="K43" s="173" t="s">
         <v>142</v>
       </c>
-      <c r="L43" s="69" t="s">
-        <v>74</v>
-      </c>
-      <c r="M43" s="154"/>
-      <c r="N43" s="196"/>
-      <c r="O43" s="196"/>
+      <c r="L43" s="68" t="s">
+        <v>74</v>
+      </c>
+      <c r="M43" s="152"/>
+      <c r="N43" s="194"/>
+      <c r="O43" s="194"/>
     </row>
     <row r="44" spans="1:15" ht="15.6" thickBot="1">
-      <c r="A44" s="88" t="s">
+      <c r="A44" s="87" t="s">
         <v>55</v>
       </c>
-      <c r="B44" s="127" t="s">
-        <v>24</v>
-      </c>
-      <c r="C44" s="155" t="s">
-        <v>82</v>
-      </c>
-      <c r="D44" s="70" t="s">
-        <v>71</v>
-      </c>
-      <c r="E44" s="176" t="s">
+      <c r="B44" s="126" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="153" t="s">
+        <v>82</v>
+      </c>
+      <c r="D44" s="69" t="s">
+        <v>71</v>
+      </c>
+      <c r="E44" s="174" t="s">
         <v>147</v>
       </c>
-      <c r="F44" s="70" t="s">
+      <c r="F44" s="69" t="s">
         <v>77</v>
       </c>
-      <c r="G44" s="176" t="s">
+      <c r="G44" s="174" t="s">
         <v>143</v>
       </c>
-      <c r="H44" s="70" t="s">
-        <v>72</v>
-      </c>
-      <c r="I44" s="155" t="s">
-        <v>73</v>
-      </c>
-      <c r="J44" s="70" t="s">
-        <v>116</v>
-      </c>
-      <c r="K44" s="176" t="s">
+      <c r="H44" s="69" t="s">
+        <v>72</v>
+      </c>
+      <c r="I44" s="153" t="s">
+        <v>73</v>
+      </c>
+      <c r="J44" s="69" t="s">
+        <v>116</v>
+      </c>
+      <c r="K44" s="174" t="s">
         <v>142</v>
       </c>
-      <c r="L44" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="M44" s="155" t="s">
+      <c r="L44" s="70" t="s">
+        <v>74</v>
+      </c>
+      <c r="M44" s="153" t="s">
         <v>101</v>
       </c>
-      <c r="N44" s="196"/>
-      <c r="O44" s="196"/>
+      <c r="N44" s="194"/>
+      <c r="O44" s="194"/>
     </row>
     <row r="45" spans="1:15" ht="15.6" thickBot="1">
-      <c r="A45" s="88" t="s">
+      <c r="A45" s="87" t="s">
         <v>56</v>
       </c>
-      <c r="B45" s="127" t="s">
-        <v>24</v>
-      </c>
-      <c r="C45" s="155" t="s">
-        <v>82</v>
-      </c>
-      <c r="D45" s="70" t="s">
-        <v>71</v>
-      </c>
-      <c r="E45" s="176" t="s">
+      <c r="B45" s="126" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" s="153" t="s">
+        <v>82</v>
+      </c>
+      <c r="D45" s="69" t="s">
+        <v>71</v>
+      </c>
+      <c r="E45" s="174" t="s">
         <v>147</v>
       </c>
-      <c r="F45" s="70" t="s">
+      <c r="F45" s="69" t="s">
         <v>77</v>
       </c>
-      <c r="G45" s="176" t="s">
+      <c r="G45" s="174" t="s">
         <v>143</v>
       </c>
-      <c r="H45" s="70" t="s">
-        <v>72</v>
-      </c>
-      <c r="I45" s="155" t="s">
-        <v>73</v>
-      </c>
-      <c r="J45" s="70" t="s">
-        <v>116</v>
-      </c>
-      <c r="K45" s="176" t="s">
+      <c r="H45" s="69" t="s">
+        <v>72</v>
+      </c>
+      <c r="I45" s="153" t="s">
+        <v>73</v>
+      </c>
+      <c r="J45" s="69" t="s">
+        <v>116</v>
+      </c>
+      <c r="K45" s="174" t="s">
         <v>142</v>
       </c>
-      <c r="L45" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="M45" s="176" t="s">
+      <c r="L45" s="70" t="s">
+        <v>74</v>
+      </c>
+      <c r="M45" s="174" t="s">
         <v>148</v>
       </c>
-      <c r="N45" s="196"/>
-      <c r="O45" s="196"/>
+      <c r="N45" s="194"/>
+      <c r="O45" s="194"/>
     </row>
     <row r="46" spans="1:15" ht="15.6" thickBot="1">
-      <c r="A46" s="88" t="s">
+      <c r="A46" s="87" t="s">
         <v>58</v>
       </c>
-      <c r="B46" s="127" t="s">
-        <v>24</v>
-      </c>
-      <c r="C46" s="155" t="s">
-        <v>82</v>
-      </c>
-      <c r="D46" s="70" t="s">
-        <v>71</v>
-      </c>
-      <c r="E46" s="176" t="s">
+      <c r="B46" s="126" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46" s="153" t="s">
+        <v>82</v>
+      </c>
+      <c r="D46" s="69" t="s">
+        <v>71</v>
+      </c>
+      <c r="E46" s="174" t="s">
         <v>147</v>
       </c>
-      <c r="F46" s="70" t="s">
+      <c r="F46" s="69" t="s">
         <v>77</v>
       </c>
-      <c r="G46" s="176" t="s">
+      <c r="G46" s="174" t="s">
         <v>143</v>
       </c>
-      <c r="H46" s="70" t="s">
-        <v>72</v>
-      </c>
-      <c r="I46" s="155" t="s">
-        <v>73</v>
-      </c>
-      <c r="J46" s="70" t="s">
-        <v>116</v>
-      </c>
-      <c r="K46" s="176" t="s">
+      <c r="H46" s="69" t="s">
+        <v>72</v>
+      </c>
+      <c r="I46" s="153" t="s">
+        <v>73</v>
+      </c>
+      <c r="J46" s="69" t="s">
+        <v>116</v>
+      </c>
+      <c r="K46" s="174" t="s">
         <v>142</v>
       </c>
-      <c r="L46" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="M46" s="155" t="s">
+      <c r="L46" s="70" t="s">
+        <v>74</v>
+      </c>
+      <c r="M46" s="153" t="s">
         <v>102</v>
       </c>
-      <c r="N46" s="196"/>
-      <c r="O46" s="196"/>
+      <c r="N46" s="194"/>
+      <c r="O46" s="194"/>
     </row>
     <row r="47" spans="1:15" ht="15.6" thickBot="1">
-      <c r="A47" s="88" t="s">
+      <c r="A47" s="87" t="s">
         <v>57</v>
       </c>
-      <c r="B47" s="127" t="s">
-        <v>24</v>
-      </c>
-      <c r="C47" s="155" t="s">
-        <v>82</v>
-      </c>
-      <c r="D47" s="70" t="s">
-        <v>71</v>
-      </c>
-      <c r="E47" s="176" t="s">
+      <c r="B47" s="126" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="153" t="s">
+        <v>82</v>
+      </c>
+      <c r="D47" s="69" t="s">
+        <v>71</v>
+      </c>
+      <c r="E47" s="174" t="s">
         <v>147</v>
       </c>
-      <c r="F47" s="70" t="s">
+      <c r="F47" s="69" t="s">
         <v>77</v>
       </c>
-      <c r="G47" s="176" t="s">
+      <c r="G47" s="174" t="s">
         <v>143</v>
       </c>
-      <c r="H47" s="70" t="s">
-        <v>72</v>
-      </c>
-      <c r="I47" s="155" t="s">
-        <v>73</v>
-      </c>
-      <c r="J47" s="70" t="s">
-        <v>116</v>
-      </c>
-      <c r="K47" s="176" t="s">
+      <c r="H47" s="69" t="s">
+        <v>72</v>
+      </c>
+      <c r="I47" s="153" t="s">
+        <v>73</v>
+      </c>
+      <c r="J47" s="69" t="s">
+        <v>116</v>
+      </c>
+      <c r="K47" s="174" t="s">
         <v>142</v>
       </c>
-      <c r="L47" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="M47" s="155" t="s">
+      <c r="L47" s="70" t="s">
+        <v>74</v>
+      </c>
+      <c r="M47" s="153" t="s">
         <v>103</v>
       </c>
-      <c r="N47" s="196"/>
-      <c r="O47" s="196"/>
+      <c r="N47" s="194"/>
+      <c r="O47" s="194"/>
     </row>
     <row r="48" spans="1:15" ht="15.6" thickBot="1">
-      <c r="A48" s="92" t="s">
+      <c r="A48" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="B48" s="128" t="s">
-        <v>24</v>
-      </c>
-      <c r="C48" s="156" t="s">
-        <v>82</v>
-      </c>
-      <c r="D48" s="72" t="s">
-        <v>71</v>
-      </c>
-      <c r="E48" s="177" t="s">
+      <c r="B48" s="127" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="154" t="s">
+        <v>82</v>
+      </c>
+      <c r="D48" s="71" t="s">
+        <v>71</v>
+      </c>
+      <c r="E48" s="175" t="s">
         <v>147</v>
       </c>
-      <c r="F48" s="72" t="s">
+      <c r="F48" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="G48" s="177" t="s">
+      <c r="G48" s="175" t="s">
         <v>143</v>
       </c>
-      <c r="H48" s="72" t="s">
-        <v>72</v>
-      </c>
-      <c r="I48" s="156" t="s">
-        <v>73</v>
-      </c>
-      <c r="J48" s="72" t="s">
-        <v>116</v>
-      </c>
-      <c r="K48" s="177" t="s">
+      <c r="H48" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="I48" s="154" t="s">
+        <v>73</v>
+      </c>
+      <c r="J48" s="71" t="s">
+        <v>116</v>
+      </c>
+      <c r="K48" s="175" t="s">
         <v>142</v>
       </c>
-      <c r="L48" s="73" t="s">
-        <v>74</v>
-      </c>
-      <c r="M48" s="156" t="s">
+      <c r="L48" s="72" t="s">
+        <v>74</v>
+      </c>
+      <c r="M48" s="154" t="s">
         <v>104</v>
       </c>
-      <c r="N48" s="197"/>
-      <c r="O48" s="197"/>
-    </row>
-    <row r="49" spans="1:13" ht="15" hidden="1">
-      <c r="A49" s="90" t="s">
+      <c r="N48" s="195"/>
+      <c r="O48" s="195"/>
+    </row>
+    <row r="49" spans="1:13" ht="15">
+      <c r="A49" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="B49" s="129" t="s">
+      <c r="B49" s="128" t="s">
         <v>60</v>
       </c>
-      <c r="C49" s="157" t="s">
-        <v>82</v>
-      </c>
-      <c r="D49" s="74" t="s">
-        <v>71</v>
-      </c>
-      <c r="E49" s="157">
+      <c r="C49" s="155" t="s">
+        <v>82</v>
+      </c>
+      <c r="D49" s="73" t="s">
+        <v>71</v>
+      </c>
+      <c r="E49" s="155">
         <v>10101991</v>
       </c>
-      <c r="F49" s="74" t="s">
+      <c r="F49" s="73" t="s">
         <v>77</v>
       </c>
-      <c r="G49" s="157">
+      <c r="G49" s="155">
         <v>11202</v>
       </c>
-      <c r="H49" s="74" t="s">
-        <v>72</v>
-      </c>
-      <c r="I49" s="157" t="s">
-        <v>73</v>
-      </c>
-      <c r="J49" s="74" t="s">
-        <v>116</v>
-      </c>
-      <c r="K49" s="157">
+      <c r="H49" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="I49" s="155" t="s">
+        <v>73</v>
+      </c>
+      <c r="J49" s="73" t="s">
+        <v>116</v>
+      </c>
+      <c r="K49" s="155">
         <v>9728657793</v>
       </c>
-      <c r="L49" s="75" t="s">
-        <v>74</v>
-      </c>
-      <c r="M49" s="157" t="s">
+      <c r="L49" s="74" t="s">
+        <v>74</v>
+      </c>
+      <c r="M49" s="155" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="15" hidden="1">
-      <c r="A50" s="89" t="s">
+    <row r="50" spans="1:13" ht="15">
+      <c r="A50" s="88" t="s">
         <v>107</v>
       </c>
-      <c r="B50" s="130" t="s">
+      <c r="B50" s="129" t="s">
         <v>60</v>
       </c>
-      <c r="C50" s="158" t="s">
-        <v>82</v>
-      </c>
-      <c r="D50" s="76" t="s">
-        <v>71</v>
-      </c>
-      <c r="E50" s="158">
+      <c r="C50" s="156" t="s">
+        <v>82</v>
+      </c>
+      <c r="D50" s="75" t="s">
+        <v>71</v>
+      </c>
+      <c r="E50" s="156">
         <v>10101991</v>
       </c>
-      <c r="F50" s="76" t="s">
+      <c r="F50" s="75" t="s">
         <v>77</v>
       </c>
-      <c r="G50" s="158">
+      <c r="G50" s="156">
         <v>11202</v>
       </c>
-      <c r="H50" s="76" t="s">
-        <v>72</v>
-      </c>
-      <c r="I50" s="158" t="s">
-        <v>73</v>
-      </c>
-      <c r="J50" s="76" t="s">
-        <v>116</v>
-      </c>
-      <c r="K50" s="158">
+      <c r="H50" s="75" t="s">
+        <v>72</v>
+      </c>
+      <c r="I50" s="156" t="s">
+        <v>73</v>
+      </c>
+      <c r="J50" s="75" t="s">
+        <v>116</v>
+      </c>
+      <c r="K50" s="156">
         <v>9728657793</v>
       </c>
-      <c r="L50" s="77" t="s">
-        <v>74</v>
-      </c>
-      <c r="M50" s="158" t="s">
+      <c r="L50" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="M50" s="156" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="15" hidden="1">
-      <c r="A51" s="89" t="s">
+    <row r="51" spans="1:13" ht="15">
+      <c r="A51" s="88" t="s">
         <v>109</v>
       </c>
-      <c r="B51" s="130" t="s">
+      <c r="B51" s="129" t="s">
         <v>60</v>
       </c>
-      <c r="C51" s="158" t="s">
-        <v>82</v>
-      </c>
-      <c r="D51" s="76" t="s">
-        <v>71</v>
-      </c>
-      <c r="E51" s="158">
+      <c r="C51" s="156" t="s">
+        <v>82</v>
+      </c>
+      <c r="D51" s="75" t="s">
+        <v>71</v>
+      </c>
+      <c r="E51" s="156">
         <v>10101991</v>
       </c>
-      <c r="F51" s="76" t="s">
+      <c r="F51" s="75" t="s">
         <v>77</v>
       </c>
-      <c r="G51" s="158">
+      <c r="G51" s="156">
         <v>11202</v>
       </c>
-      <c r="H51" s="76" t="s">
-        <v>72</v>
-      </c>
-      <c r="I51" s="158" t="s">
-        <v>73</v>
-      </c>
-      <c r="J51" s="76" t="s">
-        <v>116</v>
-      </c>
-      <c r="K51" s="158">
+      <c r="H51" s="75" t="s">
+        <v>72</v>
+      </c>
+      <c r="I51" s="156" t="s">
+        <v>73</v>
+      </c>
+      <c r="J51" s="75" t="s">
+        <v>116</v>
+      </c>
+      <c r="K51" s="156">
         <v>9728657793</v>
       </c>
-      <c r="L51" s="77" t="s">
-        <v>74</v>
-      </c>
-      <c r="M51" s="158" t="s">
+      <c r="L51" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="M51" s="156" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="30" hidden="1">
-      <c r="A52" s="89" t="s">
+    <row r="52" spans="1:13" ht="30">
+      <c r="A52" s="88" t="s">
         <v>111</v>
       </c>
-      <c r="B52" s="130" t="s">
+      <c r="B52" s="129" t="s">
         <v>60</v>
       </c>
-      <c r="C52" s="158" t="s">
-        <v>82</v>
-      </c>
-      <c r="D52" s="76" t="s">
-        <v>71</v>
-      </c>
-      <c r="E52" s="158">
+      <c r="C52" s="156" t="s">
+        <v>82</v>
+      </c>
+      <c r="D52" s="75" t="s">
+        <v>71</v>
+      </c>
+      <c r="E52" s="156">
         <v>10101991</v>
       </c>
-      <c r="F52" s="76" t="s">
+      <c r="F52" s="75" t="s">
         <v>77</v>
       </c>
-      <c r="G52" s="158">
+      <c r="G52" s="156">
         <v>11202</v>
       </c>
-      <c r="H52" s="76" t="s">
-        <v>72</v>
-      </c>
-      <c r="I52" s="158" t="s">
-        <v>73</v>
-      </c>
-      <c r="J52" s="76" t="s">
-        <v>116</v>
-      </c>
-      <c r="K52" s="158">
+      <c r="H52" s="75" t="s">
+        <v>72</v>
+      </c>
+      <c r="I52" s="156" t="s">
+        <v>73</v>
+      </c>
+      <c r="J52" s="75" t="s">
+        <v>116</v>
+      </c>
+      <c r="K52" s="156">
         <v>9728657793</v>
       </c>
-      <c r="L52" s="77" t="s">
-        <v>74</v>
-      </c>
-      <c r="M52" s="158" t="s">
+      <c r="L52" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="M52" s="156" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="30.6" hidden="1" thickBot="1">
-      <c r="A53" s="91" t="s">
+    <row r="53" spans="1:13" ht="30.6" thickBot="1">
+      <c r="A53" s="90" t="s">
         <v>113</v>
       </c>
-      <c r="B53" s="91" t="s">
+      <c r="B53" s="90" t="s">
         <v>60</v>
       </c>
-      <c r="C53" s="159" t="s">
-        <v>82</v>
-      </c>
-      <c r="D53" s="78" t="s">
-        <v>71</v>
-      </c>
-      <c r="E53" s="159">
+      <c r="C53" s="157" t="s">
+        <v>82</v>
+      </c>
+      <c r="D53" s="77" t="s">
+        <v>71</v>
+      </c>
+      <c r="E53" s="157">
         <v>10101991</v>
       </c>
-      <c r="F53" s="78" t="s">
+      <c r="F53" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="G53" s="159">
+      <c r="G53" s="157">
         <v>11202</v>
       </c>
-      <c r="H53" s="78" t="s">
-        <v>72</v>
-      </c>
-      <c r="I53" s="159" t="s">
-        <v>73</v>
-      </c>
-      <c r="J53" s="78" t="s">
-        <v>116</v>
-      </c>
-      <c r="K53" s="159">
+      <c r="H53" s="77" t="s">
+        <v>72</v>
+      </c>
+      <c r="I53" s="157" t="s">
+        <v>73</v>
+      </c>
+      <c r="J53" s="77" t="s">
+        <v>116</v>
+      </c>
+      <c r="K53" s="157">
         <v>9728657793</v>
       </c>
-      <c r="L53" s="79" t="s">
-        <v>74</v>
-      </c>
-      <c r="M53" s="159" t="s">
+      <c r="L53" s="78" t="s">
+        <v>74</v>
+      </c>
+      <c r="M53" s="157" t="s">
         <v>114</v>
       </c>
     </row>
@@ -4277,56 +4271,55 @@
     <hyperlink ref="L3" r:id="rId3"/>
     <hyperlink ref="L4" r:id="rId4"/>
     <hyperlink ref="L5" r:id="rId5"/>
-    <hyperlink ref="C4" r:id="rId6"/>
-    <hyperlink ref="L6" r:id="rId7"/>
-    <hyperlink ref="L7" r:id="rId8"/>
-    <hyperlink ref="L8" r:id="rId9"/>
-    <hyperlink ref="L9" r:id="rId10"/>
-    <hyperlink ref="D8" r:id="rId11"/>
-    <hyperlink ref="L10" r:id="rId12"/>
-    <hyperlink ref="L11" r:id="rId13"/>
-    <hyperlink ref="L12" r:id="rId14"/>
-    <hyperlink ref="L13" r:id="rId15"/>
-    <hyperlink ref="L14" r:id="rId16"/>
-    <hyperlink ref="L15" r:id="rId17"/>
-    <hyperlink ref="L16" r:id="rId18"/>
-    <hyperlink ref="L17" r:id="rId19"/>
-    <hyperlink ref="L18" r:id="rId20"/>
-    <hyperlink ref="L19" r:id="rId21"/>
-    <hyperlink ref="L20" r:id="rId22"/>
-    <hyperlink ref="L21" r:id="rId23"/>
-    <hyperlink ref="L22" r:id="rId24"/>
-    <hyperlink ref="L23" r:id="rId25"/>
-    <hyperlink ref="L24" r:id="rId26"/>
-    <hyperlink ref="L25" r:id="rId27"/>
-    <hyperlink ref="L26" r:id="rId28"/>
-    <hyperlink ref="L27" r:id="rId29"/>
-    <hyperlink ref="H26" r:id="rId30"/>
-    <hyperlink ref="L28" r:id="rId31"/>
-    <hyperlink ref="L29" r:id="rId32"/>
-    <hyperlink ref="L30" r:id="rId33"/>
-    <hyperlink ref="L31" r:id="rId34"/>
-    <hyperlink ref="L32" r:id="rId35"/>
-    <hyperlink ref="L33" r:id="rId36"/>
-    <hyperlink ref="L34" r:id="rId37"/>
-    <hyperlink ref="L35" r:id="rId38"/>
-    <hyperlink ref="L36" r:id="rId39"/>
-    <hyperlink ref="L37" r:id="rId40"/>
-    <hyperlink ref="L38" r:id="rId41"/>
-    <hyperlink ref="L39" r:id="rId42"/>
-    <hyperlink ref="L41" r:id="rId43" display="xyz987@gmail.com"/>
-    <hyperlink ref="L42" r:id="rId44"/>
-    <hyperlink ref="L43" r:id="rId45"/>
-    <hyperlink ref="L44" r:id="rId46"/>
-    <hyperlink ref="L45" r:id="rId47"/>
-    <hyperlink ref="L46" r:id="rId48"/>
-    <hyperlink ref="L47" r:id="rId49"/>
-    <hyperlink ref="L48" r:id="rId50"/>
-    <hyperlink ref="L51" r:id="rId51"/>
-    <hyperlink ref="L52" r:id="rId52"/>
-    <hyperlink ref="L50" r:id="rId53"/>
-    <hyperlink ref="L49" r:id="rId54"/>
-    <hyperlink ref="L53" r:id="rId55"/>
+    <hyperlink ref="L6" r:id="rId6"/>
+    <hyperlink ref="L7" r:id="rId7"/>
+    <hyperlink ref="L8" r:id="rId8"/>
+    <hyperlink ref="L9" r:id="rId9"/>
+    <hyperlink ref="D8" r:id="rId10"/>
+    <hyperlink ref="L10" r:id="rId11"/>
+    <hyperlink ref="L11" r:id="rId12"/>
+    <hyperlink ref="L12" r:id="rId13"/>
+    <hyperlink ref="L13" r:id="rId14"/>
+    <hyperlink ref="L14" r:id="rId15"/>
+    <hyperlink ref="L15" r:id="rId16"/>
+    <hyperlink ref="L16" r:id="rId17"/>
+    <hyperlink ref="L17" r:id="rId18"/>
+    <hyperlink ref="L18" r:id="rId19"/>
+    <hyperlink ref="L19" r:id="rId20"/>
+    <hyperlink ref="L20" r:id="rId21"/>
+    <hyperlink ref="L21" r:id="rId22"/>
+    <hyperlink ref="L22" r:id="rId23"/>
+    <hyperlink ref="L23" r:id="rId24"/>
+    <hyperlink ref="L24" r:id="rId25"/>
+    <hyperlink ref="L25" r:id="rId26"/>
+    <hyperlink ref="L26" r:id="rId27"/>
+    <hyperlink ref="L27" r:id="rId28"/>
+    <hyperlink ref="H26" r:id="rId29"/>
+    <hyperlink ref="L28" r:id="rId30"/>
+    <hyperlink ref="L29" r:id="rId31"/>
+    <hyperlink ref="L30" r:id="rId32"/>
+    <hyperlink ref="L31" r:id="rId33"/>
+    <hyperlink ref="L32" r:id="rId34"/>
+    <hyperlink ref="L33" r:id="rId35"/>
+    <hyperlink ref="L34" r:id="rId36"/>
+    <hyperlink ref="L35" r:id="rId37"/>
+    <hyperlink ref="L36" r:id="rId38"/>
+    <hyperlink ref="L37" r:id="rId39"/>
+    <hyperlink ref="L38" r:id="rId40"/>
+    <hyperlink ref="L39" r:id="rId41"/>
+    <hyperlink ref="L41" r:id="rId42" display="xyz987@gmail.com"/>
+    <hyperlink ref="L42" r:id="rId43"/>
+    <hyperlink ref="L43" r:id="rId44"/>
+    <hyperlink ref="L44" r:id="rId45"/>
+    <hyperlink ref="L45" r:id="rId46"/>
+    <hyperlink ref="L46" r:id="rId47"/>
+    <hyperlink ref="L47" r:id="rId48"/>
+    <hyperlink ref="L48" r:id="rId49"/>
+    <hyperlink ref="L51" r:id="rId50"/>
+    <hyperlink ref="L52" r:id="rId51"/>
+    <hyperlink ref="L50" r:id="rId52"/>
+    <hyperlink ref="L49" r:id="rId53"/>
+    <hyperlink ref="L53" r:id="rId54"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>